<commit_message>
Results for Modulo IK
</commit_message>
<xml_diff>
--- a/results-modulo/Results-Modulo-IK.xlsx
+++ b/results-modulo/Results-Modulo-IK.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cf2ea51ea12e088c/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cf2ea51ea12e088c/Documents/CMU/22Spring/16711/Project/results-modulo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{BA48E3C2-3329-4036-8894-DAC1B2A91729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35F0F33F-9251-4D0E-84A8-675C4C6E8123}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{BA48E3C2-3329-4036-8894-DAC1B2A91729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78E9DBD1-3696-4E04-9813-7B3FB8B5C349}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{1566B33F-8A07-4D7E-B5A1-D24689441796}"/>
+    <workbookView xWindow="368" yWindow="368" windowWidth="16365" windowHeight="14122" xr2:uid="{1566B33F-8A07-4D7E-B5A1-D24689441796}"/>
   </bookViews>
   <sheets>
     <sheet name="results (2)" sheetId="3" r:id="rId1"/>
@@ -338,11 +338,16 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AC1DC114-6646-4605-8964-8B79666FF74D}" name="results__2" displayName="results__2" ref="A1:F37" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:F37" xr:uid="{AC1DC114-6646-4605-8964-8B79666FF74D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F37">
+    <sortCondition ref="B2:B37"/>
+    <sortCondition ref="C2:C37"/>
+    <sortCondition ref="D2:D37"/>
+  </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7831F0EB-8523-46C1-8113-79466DEED054}" uniqueName="1" name="Source.Name" queryTableFieldId="1" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{63569140-720C-4DA5-82F2-8DE678B7BC47}" uniqueName="2" name="Column1" queryTableFieldId="2" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{470EDB69-514B-4F98-933D-F537FCC850DD}" uniqueName="3" name="Column2" queryTableFieldId="3" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{7A7209B9-75B2-4BF2-8A10-10D9E597106D}" uniqueName="4" name="Column3" queryTableFieldId="4" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{7831F0EB-8523-46C1-8113-79466DEED054}" uniqueName="1" name="Source.Name" queryTableFieldId="1" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{63569140-720C-4DA5-82F2-8DE678B7BC47}" uniqueName="2" name="Column1" queryTableFieldId="2" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{470EDB69-514B-4F98-933D-F537FCC850DD}" uniqueName="3" name="Column2" queryTableFieldId="3" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{7A7209B9-75B2-4BF2-8A10-10D9E597106D}" uniqueName="4" name="Column3" queryTableFieldId="4" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{6E6A06DF-58E2-4217-8B23-EAC0003517ED}" uniqueName="5" name="Column4" queryTableFieldId="5"/>
     <tableColumn id="6" xr3:uid="{C5742372-58B6-4F28-926D-FB41BD1E8806}" uniqueName="6" name="Column5" queryTableFieldId="6"/>
   </tableColumns>
@@ -354,7 +359,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3918FE9F-AB01-4D6F-B3B9-C2C72F63B6A5}" name="results" displayName="results" ref="A1:A39" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:A39" xr:uid="{3918FE9F-AB01-4D6F-B3B9-C2C72F63B6A5}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{FF9A7109-8AE6-43BB-8AEE-1C9026B28CEF}" uniqueName="1" name="Source.Name" queryTableFieldId="1" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{FF9A7109-8AE6-43BB-8AEE-1C9026B28CEF}" uniqueName="1" name="Source.Name" queryTableFieldId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -660,7 +665,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -692,110 +697,110 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E2">
-        <v>0.57689999999999997</v>
+        <v>0.55679999999999996</v>
       </c>
       <c r="F2">
-        <v>3.56E-2</v>
+        <v>3.39E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E3">
-        <v>1.1534</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>5.9700000000000003E-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E4">
-        <v>0.17199999999999999</v>
+        <v>0.62029999999999996</v>
       </c>
       <c r="F4">
-        <v>2.1600000000000001E-2</v>
+        <v>4.82E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E5">
-        <v>1.7769999999999999</v>
+        <v>0.64510000000000001</v>
       </c>
       <c r="F5">
-        <v>0.2228</v>
+        <v>0.1227</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E6">
-        <v>0.34720000000000001</v>
+        <v>0.92290000000000005</v>
       </c>
       <c r="F6">
-        <v>3.2399999999999998E-2</v>
+        <v>0.25719999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>17</v>
@@ -804,258 +809,258 @@
         <v>15</v>
       </c>
       <c r="E7">
-        <v>1.2747999999999999</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="F7">
-        <v>0.35160000000000002</v>
+        <v>0.13020000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E8">
-        <v>1.4318</v>
+        <v>0.51270000000000004</v>
       </c>
       <c r="F8">
-        <v>0.25119999999999998</v>
+        <v>1.4E-2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E9">
-        <v>0.85660000000000003</v>
+        <v>0.52449999999999997</v>
       </c>
       <c r="F9">
-        <v>0.159</v>
+        <v>9.4000000000000004E-3</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E10">
-        <v>0.75119999999999998</v>
+        <v>0.59250000000000003</v>
       </c>
       <c r="F10">
-        <v>4.8000000000000001E-2</v>
+        <v>6.6400000000000001E-2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E11">
-        <v>0.86770000000000003</v>
+        <v>0.59619999999999995</v>
       </c>
       <c r="F11">
-        <v>8.2199999999999995E-2</v>
+        <v>3.6700000000000003E-2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E12">
-        <v>1.8907</v>
+        <v>0.61270000000000002</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>4.3799999999999999E-2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E13">
-        <v>0.19989999999999999</v>
+        <v>0.57330000000000003</v>
       </c>
       <c r="F13">
-        <v>7.7999999999999996E-3</v>
+        <v>5.2299999999999999E-2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E14">
-        <v>0.73519999999999996</v>
+        <v>1.1268</v>
       </c>
       <c r="F14">
-        <v>8.5199999999999998E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E15">
-        <v>1.5651999999999999</v>
+        <v>1.2242999999999999</v>
       </c>
       <c r="F15">
-        <v>0.2041</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E16">
-        <v>1.8354999999999999</v>
+        <v>1.31</v>
       </c>
       <c r="F16">
-        <v>0.18410000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E17">
-        <v>1.5505</v>
+        <v>0.64980000000000004</v>
       </c>
       <c r="F17">
-        <v>0.24590000000000001</v>
+        <v>3.9199999999999999E-2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E18">
-        <v>1.4140999999999999</v>
+        <v>0.5827</v>
       </c>
       <c r="F18">
-        <v>0.39400000000000002</v>
+        <v>5.3199999999999997E-2</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E19">
-        <v>0.34339999999999998</v>
+        <v>0.60399999999999998</v>
       </c>
       <c r="F19">
-        <v>5.2600000000000001E-2</v>
+        <v>3.09E-2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>17</v>
@@ -1064,278 +1069,278 @@
         <v>13</v>
       </c>
       <c r="E20">
-        <v>0.55679999999999996</v>
+        <v>0.34720000000000001</v>
       </c>
       <c r="F20">
-        <v>3.39E-2</v>
+        <v>3.2399999999999998E-2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E21">
-        <v>0.92290000000000005</v>
+        <v>0.34339999999999998</v>
       </c>
       <c r="F21">
-        <v>0.25719999999999998</v>
+        <v>5.2600000000000001E-2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E22">
-        <v>1.31</v>
+        <v>0.75119999999999998</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>4.8000000000000001E-2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E23">
-        <v>0.57499999999999996</v>
+        <v>0.86770000000000003</v>
       </c>
       <c r="F23">
-        <v>5.9700000000000003E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E24">
-        <v>0.5827</v>
+        <v>1.2747999999999999</v>
       </c>
       <c r="F24">
-        <v>5.3199999999999997E-2</v>
+        <v>0.35160000000000002</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E25">
-        <v>0.51270000000000004</v>
+        <v>0.73519999999999996</v>
       </c>
       <c r="F25">
-        <v>1.4E-2</v>
+        <v>8.5199999999999998E-2</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E26">
-        <v>1.1268</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>2.1600000000000001E-2</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E27">
-        <v>0.66669999999999996</v>
+        <v>0.19989999999999999</v>
       </c>
       <c r="F27">
-        <v>0.13020000000000001</v>
+        <v>7.7999999999999996E-3</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E28">
-        <v>0.60399999999999998</v>
+        <v>0.57689999999999997</v>
       </c>
       <c r="F28">
-        <v>3.09E-2</v>
+        <v>3.56E-2</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E29">
-        <v>0.61270000000000002</v>
+        <v>1.5505</v>
       </c>
       <c r="F29">
-        <v>4.3799999999999999E-2</v>
+        <v>0.24590000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E30">
-        <v>0.59250000000000003</v>
+        <v>1.7769999999999999</v>
       </c>
       <c r="F30">
-        <v>6.6400000000000001E-2</v>
+        <v>0.2228</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E31">
-        <v>0.59619999999999995</v>
+        <v>1.4140999999999999</v>
       </c>
       <c r="F31">
-        <v>3.6700000000000003E-2</v>
+        <v>0.39400000000000002</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E32">
-        <v>0.62029999999999996</v>
+        <v>0.85660000000000003</v>
       </c>
       <c r="F32">
-        <v>4.82E-2</v>
+        <v>0.159</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E33">
-        <v>0.64510000000000001</v>
+        <v>1.8907</v>
       </c>
       <c r="F33">
-        <v>0.1227</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>11</v>
@@ -1344,70 +1349,70 @@
         <v>9</v>
       </c>
       <c r="E34">
-        <v>0.64980000000000004</v>
+        <v>1.1534</v>
       </c>
       <c r="F34">
-        <v>3.9199999999999999E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E35">
-        <v>0.57330000000000003</v>
+        <v>1.5651999999999999</v>
       </c>
       <c r="F35">
-        <v>5.2299999999999999E-2</v>
+        <v>0.2041</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E36">
-        <v>1.2242999999999999</v>
+        <v>1.4318</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>0.25119999999999998</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E37">
-        <v>0.52449999999999997</v>
+        <v>1.8354999999999999</v>
       </c>
       <c r="F37">
-        <v>9.4000000000000004E-3</v>
+        <v>0.18410000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>